<commit_message>
cal 2 & 7
</commit_message>
<xml_diff>
--- a/Saves/F2V_Cal20180104.xlsx
+++ b/Saves/F2V_Cal20180104.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Freq, Hz</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>SN5 rept</t>
+  </si>
+  <si>
+    <t>SN2?</t>
+  </si>
+  <si>
+    <t>SN7?</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SN2</c:v>
+                  <c:v>SN2?</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2092,7 +2098,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SN2</c:v>
+                  <c:v>SN2?</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2665,7 +2671,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>SN7</c:v>
+                        <c:v>SN7?</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -5169,10 +5175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5183,9 +5189,10 @@
     <col min="4" max="4" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="12" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5208,7 +5215,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>22</v>
@@ -5223,7 +5230,7 @@
         <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
@@ -5249,8 +5256,17 @@
       <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>150</v>
       </c>
@@ -5318,8 +5334,17 @@
       <c r="U2" s="1">
         <v>0.64400000000000002</v>
       </c>
+      <c r="V2" s="1">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="X2" s="1">
+        <v>150</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -5385,8 +5410,17 @@
       <c r="U3" s="1">
         <v>0.85499999999999998</v>
       </c>
+      <c r="V3" s="1">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="X3" s="1">
+        <v>200</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>300</v>
       </c>
@@ -5452,8 +5486,17 @@
       <c r="U4" s="1">
         <v>1.278</v>
       </c>
+      <c r="V4" s="1">
+        <v>1.1111</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="X4" s="1">
+        <v>300</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>400</v>
       </c>
@@ -5521,8 +5564,17 @@
       <c r="U5" s="1">
         <v>1.6970000000000001</v>
       </c>
+      <c r="V5" s="1">
+        <v>1.58</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1.476</v>
+      </c>
+      <c r="X5" s="1">
+        <v>400</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>450</v>
       </c>
@@ -5588,8 +5640,17 @@
       <c r="U6" s="1">
         <v>1.9039999999999999</v>
       </c>
+      <c r="V6" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1.81</v>
+      </c>
+      <c r="X6" s="1">
+        <v>450</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>500</v>
       </c>
@@ -5655,8 +5716,17 @@
       <c r="U7" s="1">
         <v>2.1</v>
       </c>
+      <c r="V7" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1.97</v>
+      </c>
+      <c r="X7" s="1">
+        <v>500</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>550</v>
       </c>
@@ -5722,8 +5792,17 @@
       <c r="U8" s="1">
         <v>2.29</v>
       </c>
+      <c r="V8" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="W8" s="1">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="X8" s="1">
+        <v>550</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>600</v>
       </c>
@@ -5791,8 +5870,17 @@
       <c r="U9" s="1">
         <v>2.4900000000000002</v>
       </c>
+      <c r="V9" s="1">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="W9" s="1">
+        <v>2.36</v>
+      </c>
+      <c r="X9" s="1">
+        <v>600</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>650</v>
       </c>
@@ -5858,12 +5946,21 @@
       <c r="U10" s="1">
         <v>2.69</v>
       </c>
+      <c r="V10" s="1">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="W10" s="1">
+        <v>2.46</v>
+      </c>
+      <c r="X10" s="1">
+        <v>650</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -5889,12 +5986,21 @@
       <c r="U12" s="1">
         <v>4.8</v>
       </c>
+      <c r="V12" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="W12" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -5932,7 +6038,7 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -5970,7 +6076,7 @@
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
@@ -6008,13 +6114,13 @@
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M17" s="1">
         <v>5.12</v>
       </c>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>150</v>
       </c>
@@ -6037,32 +6143,35 @@
         <v>0.05</v>
       </c>
       <c r="O18" s="1"/>
+      <c r="X18" s="1">
+        <v>150</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>

</xml_diff>

<commit_message>
error analysis of f2v data
</commit_message>
<xml_diff>
--- a/Saves/F2V_Cal20180104.xlsx
+++ b/Saves/F2V_Cal20180104.xlsx
@@ -4,28 +4,29 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary V4" sheetId="2" r:id="rId1"/>
     <sheet name="Chart1" sheetId="3" r:id="rId2"/>
-    <sheet name="Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Data" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">Data!#REF!</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Data!#REF!</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>Freq, Hz</t>
   </si>
@@ -143,6 +144,105 @@
   <si>
     <t>saturation, vrms.     Not measureable because signal generator does not produce enough voltage to satureate the LM2907/LM2917 device.</t>
   </si>
+  <si>
+    <t>SN_0-1-3-4-5-5r-6_5</t>
+  </si>
+  <si>
+    <t>uncertainties</t>
+  </si>
+  <si>
+    <t>voltage 5v regulator +/-0.1 vdc</t>
+  </si>
+  <si>
+    <t>+/- % pt</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
+  <si>
+    <t>PROBABILITY OUTPUT</t>
+  </si>
+  <si>
+    <t>Percentile</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Data scatter +/-0.1 v@3</t>
+  </si>
 </sst>
 </file>
 
@@ -150,10 +250,18 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,7 +277,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -177,11 +285,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,11 +323,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,11 +1254,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198179312"/>
-        <c:axId val="198181272"/>
+        <c:axId val="190499608"/>
+        <c:axId val="97464424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198179312"/>
+        <c:axId val="190499608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,12 +1338,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198181272"/>
+        <c:crossAx val="97464424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198181272"/>
+        <c:axId val="97464424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198179312"/>
+        <c:crossAx val="190499608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2423,11 +2561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="510994496"/>
-        <c:axId val="510983520"/>
+        <c:axId val="505695800"/>
+        <c:axId val="505691096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="510994496"/>
+        <c:axId val="505695800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2484,12 +2622,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510983520"/>
+        <c:crossAx val="505691096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="510983520"/>
+        <c:axId val="505691096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,7 +2684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510994496"/>
+        <c:crossAx val="505695800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3476,8 +3614,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198178528"/>
-        <c:axId val="198176960"/>
+        <c:axId val="505696192"/>
+        <c:axId val="505695016"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3618,7 +3756,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198178528"/>
+        <c:axId val="505696192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,12 +3874,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198176960"/>
+        <c:crossAx val="505695016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198176960"/>
+        <c:axId val="505695016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3861,7 +3999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198178528"/>
+        <c:crossAx val="505696192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3905,6 +4043,867 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fit to SN 0, 1, 3, 4, 5, 5r, 6</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AJ$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RPM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>SN_0-1-3-4-5-5r-6</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:backward val="0.70000000000000007"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10552865266841645"/>
+                  <c:y val="8.8425925925925929E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$AI$2:$AI$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>0.67187500000000011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89687500000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3427083333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.78125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9895833333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2083333333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.395833333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6145833333333335</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8125000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68958333333333344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.92083333333333339</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0416666666666665</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2708333333333335</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.46875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6979166666666665</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.885416666666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.67500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3468749999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7916666666666667</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.21875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4270833333333335</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.635416666666667</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.8020833333333335</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.69062500000000016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.921875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3791666666666669</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.052083333333333</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2708333333333335</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.479166666666667</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.7083333333333339</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.916666666666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.66145833333333337</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.87916666666666665</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.3177083333333335</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.7416666666666667</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.9562499999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.34375</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.5416666666666665</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.7395833333333335</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.67083333333333339</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.890625</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.3312500000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7677083333333334</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.1875000000000004</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.385416666666667</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.59375</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.8020833333333335</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.6635416666666667</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.88437500000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.3229166666666667</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.7593750000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.9729166666666667</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.1770833333333335</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.3645833333333335</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.572916666666667</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.78125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$AJ$2:$AJ$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>39000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="519654760"/>
+        <c:axId val="509264856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="519654760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>v4, volts normed to 5 v</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509264856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="509264856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nt,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> rpm</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="519654760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4062,6 +5061,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5095,6 +6134,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5625,7 +7180,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5713,6 +7268,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6008,10 +7593,757 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG25"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView topLeftCell="K10" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.99975164058694566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.99950334285628939</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.98337431059822489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="9">
+        <v>611.10893437582445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>46596845843.960213</v>
+      </c>
+      <c r="D12" s="9">
+        <v>46596845843.960213</v>
+      </c>
+      <c r="E12" s="9">
+        <v>124772.60831107054</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1.0520747078853019E-102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="9">
+        <v>62</v>
+      </c>
+      <c r="C13" s="9">
+        <v>23154156.039785251</v>
+      </c>
+      <c r="D13" s="9">
+        <v>373454.12967395567</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="10">
+        <v>63</v>
+      </c>
+      <c r="C14" s="10">
+        <v>46620000000</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I17" s="9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="10">
+        <v>13632.38227201082</v>
+      </c>
+      <c r="C18" s="10">
+        <v>38.593318971883164</v>
+      </c>
+      <c r="D18" s="10">
+        <v>353.23166380021831</v>
+      </c>
+      <c r="E18" s="10">
+        <v>3.8181667504792258E-104</v>
+      </c>
+      <c r="F18" s="10">
+        <v>13555.235326638242</v>
+      </c>
+      <c r="G18" s="10">
+        <v>13709.529217383399</v>
+      </c>
+      <c r="H18" s="10">
+        <v>13555.235326638242</v>
+      </c>
+      <c r="I18" s="10">
+        <v>13709.529217383399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
+        <v>0.79365079365079361</v>
+      </c>
+      <c r="B25" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
+        <v>2.3809523809523809</v>
+      </c>
+      <c r="B26" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>3.9682539682539679</v>
+      </c>
+      <c r="B27" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="B28" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="B29" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
+        <v>8.7301587301587293</v>
+      </c>
+      <c r="B30" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
+        <v>10.317460317460318</v>
+      </c>
+      <c r="B31" s="9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
+        <v>11.904761904761905</v>
+      </c>
+      <c r="B32" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>13.492063492063492</v>
+      </c>
+      <c r="B33" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="9">
+        <v>15.079365079365079</v>
+      </c>
+      <c r="B34" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="B35" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
+        <v>18.253968253968253</v>
+      </c>
+      <c r="B36" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>19.841269841269842</v>
+      </c>
+      <c r="B37" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>21.428571428571427</v>
+      </c>
+      <c r="B38" s="9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="9">
+        <v>23.015873015873016</v>
+      </c>
+      <c r="B39" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="9">
+        <v>24.603174603174601</v>
+      </c>
+      <c r="B40" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
+        <v>26.19047619047619</v>
+      </c>
+      <c r="B41" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
+        <v>27.777777777777779</v>
+      </c>
+      <c r="B42" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
+        <v>29.365079365079364</v>
+      </c>
+      <c r="B43" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
+        <v>30.952380952380953</v>
+      </c>
+      <c r="B44" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
+        <v>32.539682539682538</v>
+      </c>
+      <c r="B45" s="9">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="9">
+        <v>34.126984126984119</v>
+      </c>
+      <c r="B46" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
+        <v>35.714285714285708</v>
+      </c>
+      <c r="B47" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="9">
+        <v>37.301587301587297</v>
+      </c>
+      <c r="B48" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="9">
+        <v>38.888888888888886</v>
+      </c>
+      <c r="B49" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
+        <v>40.476190476190474</v>
+      </c>
+      <c r="B50" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
+        <v>42.063492063492056</v>
+      </c>
+      <c r="B51" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="9">
+        <v>43.650793650793645</v>
+      </c>
+      <c r="B52" s="9">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
+        <v>45.238095238095234</v>
+      </c>
+      <c r="B53" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="9">
+        <v>46.825396825396822</v>
+      </c>
+      <c r="B54" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="9">
+        <v>48.412698412698404</v>
+      </c>
+      <c r="B55" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="9">
+        <v>49.999999999999993</v>
+      </c>
+      <c r="B56" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="9">
+        <v>51.587301587301582</v>
+      </c>
+      <c r="B57" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="9">
+        <v>53.17460317460317</v>
+      </c>
+      <c r="B58" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="9">
+        <v>54.761904761904759</v>
+      </c>
+      <c r="B59" s="9">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="9">
+        <v>56.349206349206341</v>
+      </c>
+      <c r="B60" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="9">
+        <v>57.93650793650793</v>
+      </c>
+      <c r="B61" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="9">
+        <v>59.523809523809518</v>
+      </c>
+      <c r="B62" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="9">
+        <v>61.111111111111107</v>
+      </c>
+      <c r="B63" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="9">
+        <v>62.698412698412689</v>
+      </c>
+      <c r="B64" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="9">
+        <v>64.285714285714278</v>
+      </c>
+      <c r="B65" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="9">
+        <v>65.873015873015873</v>
+      </c>
+      <c r="B66" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="9">
+        <v>67.460317460317455</v>
+      </c>
+      <c r="B67" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="9">
+        <v>69.047619047619051</v>
+      </c>
+      <c r="B68" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="9">
+        <v>70.634920634920633</v>
+      </c>
+      <c r="B69" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="9">
+        <v>72.222222222222229</v>
+      </c>
+      <c r="B70" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="9">
+        <v>73.80952380952381</v>
+      </c>
+      <c r="B71" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="9">
+        <v>75.396825396825392</v>
+      </c>
+      <c r="B72" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="9">
+        <v>76.984126984126988</v>
+      </c>
+      <c r="B73" s="9">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="9">
+        <v>78.571428571428569</v>
+      </c>
+      <c r="B74" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="9">
+        <v>80.158730158730165</v>
+      </c>
+      <c r="B75" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="9">
+        <v>81.746031746031747</v>
+      </c>
+      <c r="B76" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="9">
+        <v>83.333333333333329</v>
+      </c>
+      <c r="B77" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="9">
+        <v>84.920634920634924</v>
+      </c>
+      <c r="B78" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="9">
+        <v>86.507936507936506</v>
+      </c>
+      <c r="B79" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="9">
+        <v>88.095238095238088</v>
+      </c>
+      <c r="B80" s="9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="9">
+        <v>89.682539682539684</v>
+      </c>
+      <c r="B81" s="9">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="9">
+        <v>91.269841269841265</v>
+      </c>
+      <c r="B82" s="9">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="9">
+        <v>92.857142857142861</v>
+      </c>
+      <c r="B83" s="9">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="9">
+        <v>94.444444444444443</v>
+      </c>
+      <c r="B84" s="9">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="9">
+        <v>96.031746031746025</v>
+      </c>
+      <c r="B85" s="9">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="9">
+        <v>97.61904761904762</v>
+      </c>
+      <c r="B86" s="9">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="10">
+        <v>99.206349206349202</v>
+      </c>
+      <c r="B87" s="10">
+        <v>39000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B25:B87">
+    <sortCondition ref="B25"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AP6" sqref="AP6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6024,9 +8356,11 @@
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.88671875" style="1"/>
+    <col min="37" max="37" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6126,8 +8460,14 @@
       <c r="AG1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>150</v>
       </c>
@@ -6205,57 +8545,76 @@
         <v>150</v>
       </c>
       <c r="Y2" s="5">
-        <f>O2/O$12*5</f>
+        <f t="shared" ref="Y2:Y10" si="0">O2/O$12*5</f>
         <v>0.67187500000000011</v>
       </c>
       <c r="Z2" s="5">
-        <f>P2/P$12*5</f>
+        <f t="shared" ref="Z2:Z10" si="1">P2/P$12*5</f>
         <v>0.68958333333333344</v>
       </c>
       <c r="AA2" s="5">
-        <f>Q2/Q$12*5</f>
+        <f t="shared" ref="AA2:AA10" si="2">Q2/Q$12*5</f>
         <v>0.56222222222222218</v>
       </c>
       <c r="AB2" s="5">
-        <f>R2/R$12*5</f>
+        <f t="shared" ref="AB2:AB10" si="3">R2/R$12*5</f>
         <v>0.67500000000000004</v>
       </c>
       <c r="AC2" s="5">
-        <f>S2/S$12*5</f>
+        <f t="shared" ref="AC2:AC10" si="4">S2/S$12*5</f>
         <v>0.69062500000000016</v>
       </c>
       <c r="AD2" s="5">
-        <f>T2/T$12*5</f>
+        <f t="shared" ref="AD2:AD10" si="5">T2/T$12*5</f>
         <v>0.66145833333333337</v>
       </c>
       <c r="AE2" s="5">
-        <f>U2/U$12*5</f>
+        <f t="shared" ref="AE2:AE10" si="6">U2/U$12*5</f>
         <v>0.67083333333333339</v>
       </c>
       <c r="AF2" s="5">
-        <f>V2/V$12*5</f>
+        <f t="shared" ref="AF2:AF10" si="7">V2/V$12*5</f>
         <v>0.6635416666666667</v>
       </c>
       <c r="AG2" s="5">
-        <f>W2/W$12*5</f>
+        <f t="shared" ref="AG2:AG10" si="8">W2/W$12*5</f>
         <v>0.60638297872340419</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI2">
+        <v>0.67187500000000011</v>
+      </c>
+      <c r="AJ2">
+        <v>9000</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL2" s="2">
+        <f>INDEX(LINEST($AJ$2:$AJ$64,AI$2:AI$64^{1,2},FALSE,FALSE),3)</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>200</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C10" si="0">A3*0.0281</f>
+        <f t="shared" ref="C3:C10" si="9">A3*0.0281</f>
         <v>5.62</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D10" si="1">C3/2</f>
+        <f t="shared" ref="D3:D10" si="10">C3/2</f>
         <v>2.81</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E10" si="2">D3*SQRT(2)/2</f>
+        <f t="shared" ref="E3:E10" si="11">D3*SQRT(2)/2</f>
         <v>1.9869700551341987</v>
       </c>
       <c r="F3" s="1">
@@ -6283,7 +8642,7 @@
         <v>0.93799999999999994</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N10" si="3">A3*60</f>
+        <f t="shared" ref="N3:N10" si="12">A3*60</f>
         <v>12000</v>
       </c>
       <c r="O3" s="1">
@@ -6317,57 +8676,77 @@
         <v>200</v>
       </c>
       <c r="Y3" s="5">
-        <f>O3/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>0.89687500000000009</v>
       </c>
       <c r="Z3" s="5">
-        <f>P3/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>0.92083333333333339</v>
       </c>
       <c r="AA3" s="5">
-        <f>Q3/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>0.79777777777777781</v>
       </c>
       <c r="AB3" s="5">
-        <f>R3/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="AC3" s="5">
-        <f>S3/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>0.921875</v>
       </c>
       <c r="AD3" s="5">
-        <f>T3/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>0.87916666666666665</v>
       </c>
       <c r="AE3" s="5">
-        <f>U3/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>0.890625</v>
       </c>
       <c r="AF3" s="5">
-        <f>V3/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>0.88437500000000002</v>
       </c>
       <c r="AG3" s="5">
-        <f>W3/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>0.83191489361702131</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI3">
+        <v>0.89687500000000009</v>
+      </c>
+      <c r="AJ3">
+        <v>12000</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL3" s="2">
+        <f>INDEX(LINEST($AJ$2:$AJ$64,AI$2:AI$64^{1,2},FALSE,FALSE),2)</f>
+        <v>13075.140888643438</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ3" s="8">
+        <f>0.1/5*100</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>300</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8.43</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>4.2149999999999999</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2.9804550827012979</v>
       </c>
       <c r="F4" s="1">
@@ -6395,7 +8774,7 @@
         <v>1.405</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>18000</v>
       </c>
       <c r="O4" s="1">
@@ -6429,43 +8808,63 @@
         <v>300</v>
       </c>
       <c r="Y4" s="5">
-        <f>O4/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>1.3427083333333334</v>
       </c>
       <c r="Z4" s="5">
-        <f>P4/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
       <c r="AA4" s="5">
-        <f>Q4/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>1.2345555555555556</v>
       </c>
       <c r="AB4" s="5">
-        <f>R4/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>1.3468749999999998</v>
       </c>
       <c r="AC4" s="5">
-        <f>S4/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>1.3791666666666669</v>
       </c>
       <c r="AD4" s="5">
-        <f>T4/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>1.3177083333333335</v>
       </c>
       <c r="AE4" s="5">
-        <f>U4/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>1.3312500000000003</v>
       </c>
       <c r="AF4" s="5">
-        <f>V4/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>1.3229166666666667</v>
       </c>
       <c r="AG4" s="5">
-        <f>W4/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>1.1489361702127661</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI4">
+        <v>1.3427083333333334</v>
+      </c>
+      <c r="AJ4">
+        <v>18000</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL4" s="2">
+        <f>INDEX(LINEST($AJ$2:$AJ$64,AI$2:AI$64^{1,2},FALSE,FALSE),1)</f>
+        <v>241.69450165398891</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ4" s="8">
+        <f>0.1/3*100</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>400</v>
       </c>
@@ -6473,15 +8872,15 @@
         <v>10.8</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>11.24</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>5.62</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3.9739401102683973</v>
       </c>
       <c r="F5" s="1">
@@ -6509,7 +8908,7 @@
         <v>1.8680000000000001</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>24000</v>
       </c>
       <c r="O5" s="1">
@@ -6543,57 +8942,63 @@
         <v>400</v>
       </c>
       <c r="Y5" s="5">
-        <f>O5/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>1.78125</v>
       </c>
       <c r="Z5" s="5">
-        <f>P5/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
       <c r="AA5" s="5">
-        <f>Q5/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>1.7555555555555558</v>
       </c>
       <c r="AB5" s="5">
-        <f>R5/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>1.7916666666666667</v>
       </c>
       <c r="AC5" s="5">
-        <f>S5/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>1.8333333333333335</v>
       </c>
       <c r="AD5" s="5">
-        <f>T5/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>1.7416666666666667</v>
       </c>
       <c r="AE5" s="5">
-        <f>U5/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>1.7677083333333334</v>
       </c>
       <c r="AF5" s="5">
-        <f>V5/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>1.7593750000000004</v>
       </c>
       <c r="AG5" s="5">
-        <f>W5/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>1.5702127659574465</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI5">
+        <v>1.78125</v>
+      </c>
+      <c r="AJ5">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>450</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>12.645</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>6.3224999999999998</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4.4706826240519471</v>
       </c>
       <c r="F6" s="1">
@@ -6621,7 +9026,7 @@
         <v>2.09</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>27000</v>
       </c>
       <c r="O6" s="1">
@@ -6655,57 +9060,63 @@
         <v>450</v>
       </c>
       <c r="Y6" s="5">
-        <f>O6/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>1.9895833333333333</v>
       </c>
       <c r="Z6" s="5">
-        <f>P6/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>2.0416666666666665</v>
       </c>
       <c r="AA6" s="5">
-        <f>Q6/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>1.8444444444444443</v>
       </c>
       <c r="AB6" s="5">
-        <f>R6/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AC6" s="5">
-        <f>S6/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>2.052083333333333</v>
       </c>
       <c r="AD6" s="5">
-        <f>T6/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>1.9562499999999998</v>
       </c>
       <c r="AE6" s="5">
-        <f>U6/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>1.9833333333333334</v>
       </c>
       <c r="AF6" s="5">
-        <f>V6/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>1.9729166666666667</v>
       </c>
       <c r="AG6" s="5">
-        <f>W6/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>1.925531914893617</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI6">
+        <v>1.9895833333333333</v>
+      </c>
+      <c r="AJ6">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>500</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>14.05</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>7.0250000000000004</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4.9674251378354972</v>
       </c>
       <c r="F7" s="1">
@@ -6733,7 +9144,7 @@
         <v>2.33</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>30000</v>
       </c>
       <c r="O7" s="1">
@@ -6767,57 +9178,63 @@
         <v>500</v>
       </c>
       <c r="Y7" s="5">
-        <f>O7/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>2.2083333333333335</v>
       </c>
       <c r="Z7" s="5">
-        <f>P7/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>2.2708333333333335</v>
       </c>
       <c r="AA7" s="5">
-        <f>Q7/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>2.1111111111111112</v>
       </c>
       <c r="AB7" s="5">
-        <f>R7/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>2.21875</v>
       </c>
       <c r="AC7" s="5">
-        <f>S7/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>2.2708333333333335</v>
       </c>
       <c r="AD7" s="5">
-        <f>T7/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>2.166666666666667</v>
       </c>
       <c r="AE7" s="5">
-        <f>U7/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>2.1875000000000004</v>
       </c>
       <c r="AF7" s="5">
-        <f>V7/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>2.1770833333333335</v>
       </c>
       <c r="AG7" s="5">
-        <f>W7/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>2.0957446808510638</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI7">
+        <v>2.2083333333333335</v>
+      </c>
+      <c r="AJ7">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>550</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>15.455</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>7.7275</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>5.4641676516190465</v>
       </c>
       <c r="F8" s="1">
@@ -6845,7 +9262,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>33000</v>
       </c>
       <c r="O8" s="1">
@@ -6879,43 +9296,49 @@
         <v>550</v>
       </c>
       <c r="Y8" s="5">
-        <f>O8/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>2.395833333333333</v>
       </c>
       <c r="Z8" s="5">
-        <f>P8/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>2.46875</v>
       </c>
       <c r="AA8" s="5">
-        <f>Q8/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>2.2888888888888888</v>
       </c>
       <c r="AB8" s="5">
-        <f>R8/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>2.4270833333333335</v>
       </c>
       <c r="AC8" s="5">
-        <f>S8/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>2.479166666666667</v>
       </c>
       <c r="AD8" s="5">
-        <f>T8/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>2.34375</v>
       </c>
       <c r="AE8" s="5">
-        <f>U8/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>2.385416666666667</v>
       </c>
       <c r="AF8" s="5">
-        <f>V8/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>2.3645833333333335</v>
       </c>
       <c r="AG8" s="5">
-        <f>W8/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>2.3617021276595747</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI8">
+        <v>2.395833333333333</v>
+      </c>
+      <c r="AJ8">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>600</v>
       </c>
@@ -6923,15 +9346,15 @@
         <v>17.2</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>16.86</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>8.43</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>5.9609101654025958</v>
       </c>
       <c r="F9" s="1">
@@ -6959,7 +9382,7 @@
         <v>2.78</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>36000</v>
       </c>
       <c r="O9" s="1">
@@ -6993,57 +9416,63 @@
         <v>600</v>
       </c>
       <c r="Y9" s="5">
-        <f>O9/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>2.6145833333333335</v>
       </c>
       <c r="Z9" s="5">
-        <f>P9/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>2.6979166666666665</v>
       </c>
       <c r="AA9" s="5">
-        <f>Q9/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>2.4666666666666668</v>
       </c>
       <c r="AB9" s="5">
-        <f>R9/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>2.635416666666667</v>
       </c>
       <c r="AC9" s="5">
-        <f>S9/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>2.7083333333333339</v>
       </c>
       <c r="AD9" s="5">
-        <f>T9/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>2.5416666666666665</v>
       </c>
       <c r="AE9" s="5">
-        <f>U9/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>2.59375</v>
       </c>
       <c r="AF9" s="5">
-        <f>V9/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>2.572916666666667</v>
       </c>
       <c r="AG9" s="5">
-        <f>W9/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>2.5106382978723403</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI9">
+        <v>2.6145833333333335</v>
+      </c>
+      <c r="AJ9">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>650</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>18.265000000000001</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>9.1325000000000003</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>6.4576526791861459</v>
       </c>
       <c r="F10" s="1">
@@ -7071,7 +9500,7 @@
         <v>3.01</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>39000</v>
       </c>
       <c r="O10" s="1">
@@ -7105,47 +9534,59 @@
         <v>650</v>
       </c>
       <c r="Y10" s="5">
-        <f>O10/O$12*5</f>
+        <f t="shared" si="0"/>
         <v>2.8125000000000004</v>
       </c>
       <c r="Z10" s="5">
-        <f>P10/P$12*5</f>
+        <f t="shared" si="1"/>
         <v>2.885416666666667</v>
       </c>
       <c r="AA10" s="5">
-        <f>Q10/Q$12*5</f>
+        <f t="shared" si="2"/>
         <v>2.7</v>
       </c>
       <c r="AB10" s="5">
-        <f>R10/R$12*5</f>
+        <f t="shared" si="3"/>
         <v>2.8020833333333335</v>
       </c>
       <c r="AC10" s="5">
-        <f>S10/S$12*5</f>
+        <f t="shared" si="4"/>
         <v>2.916666666666667</v>
       </c>
       <c r="AD10" s="5">
-        <f>T10/T$12*5</f>
+        <f t="shared" si="5"/>
         <v>2.7395833333333335</v>
       </c>
       <c r="AE10" s="5">
-        <f>U10/U$12*5</f>
+        <f t="shared" si="6"/>
         <v>2.8020833333333335</v>
       </c>
       <c r="AF10" s="5">
-        <f>V10/V$12*5</f>
+        <f t="shared" si="7"/>
         <v>2.78125</v>
       </c>
       <c r="AG10" s="5">
-        <f>W10/W$12*5</f>
+        <f t="shared" si="8"/>
         <v>2.6170212765957448</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI10">
+        <v>2.8125000000000004</v>
+      </c>
+      <c r="AJ10">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M11" s="1"/>
       <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI11">
+        <v>0.68958333333333344</v>
+      </c>
+      <c r="AJ11">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -7177,8 +9618,14 @@
       <c r="W12" s="1">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI12">
+        <v>0.92083333333333339</v>
+      </c>
+      <c r="AJ12">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -7198,8 +9645,14 @@
       <c r="W13" s="1">
         <v>98000</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI13">
+        <v>1.375</v>
+      </c>
+      <c r="AJ13">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -7272,8 +9725,19 @@
         <f>INDEX(LINEST($N$2:$N$10,AG$2:AG$10^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI14">
+        <v>1.8333333333333335</v>
+      </c>
+      <c r="AJ14">
+        <v>24000</v>
+      </c>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -7346,8 +9810,19 @@
         <f>INDEX(LINEST($N$2:$N$10,AG$2:AG$10^{1,2},FALSE,FALSE),2)</f>
         <v>15136.749829040513</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AI15">
+        <v>2.0416666666666665</v>
+      </c>
+      <c r="AJ15">
+        <v>27000</v>
+      </c>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
@@ -7420,14 +9895,31 @@
         <f>INDEX(LINEST($N$2:$N$10,AG$2:AG$10^{1,2},FALSE,FALSE),1)</f>
         <v>-293.79797147707922</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI16">
+        <v>2.2708333333333335</v>
+      </c>
+      <c r="AJ16">
+        <v>30000</v>
+      </c>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="M17" s="1">
         <v>5.12</v>
       </c>
       <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI17">
+        <v>2.46875</v>
+      </c>
+      <c r="AJ17">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>150</v>
       </c>
@@ -7450,8 +9942,14 @@
         <v>0.05</v>
       </c>
       <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI18">
+        <v>2.6979166666666665</v>
+      </c>
+      <c r="AJ18">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>650</v>
       </c>
@@ -7460,28 +9958,64 @@
       </c>
       <c r="M19" s="1"/>
       <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI19">
+        <v>2.885416666666667</v>
+      </c>
+      <c r="AJ19">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="M20" s="1"/>
       <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI20">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="AJ20">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="M21" s="1"/>
       <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI21">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AJ21">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="M22" s="1"/>
       <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI22">
+        <v>1.3468749999999998</v>
+      </c>
+      <c r="AJ22">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="M23" s="1"/>
       <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI23">
+        <v>1.7916666666666667</v>
+      </c>
+      <c r="AJ23">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="M24" s="1"/>
       <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="AI24">
+        <v>2</v>
+      </c>
+      <c r="AJ24">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
@@ -7489,6 +10023,324 @@
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
+      <c r="AI25">
+        <v>2.21875</v>
+      </c>
+      <c r="AJ25">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI26">
+        <v>2.4270833333333335</v>
+      </c>
+      <c r="AJ26">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI27">
+        <v>2.635416666666667</v>
+      </c>
+      <c r="AJ27">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI28">
+        <v>2.8020833333333335</v>
+      </c>
+      <c r="AJ28">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI29">
+        <v>0.69062500000000016</v>
+      </c>
+      <c r="AJ29">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI30">
+        <v>0.921875</v>
+      </c>
+      <c r="AJ30">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI31">
+        <v>1.3791666666666669</v>
+      </c>
+      <c r="AJ31">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI32">
+        <v>1.8333333333333335</v>
+      </c>
+      <c r="AJ32">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="33" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI33">
+        <v>2.052083333333333</v>
+      </c>
+      <c r="AJ33">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="34" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI34">
+        <v>2.2708333333333335</v>
+      </c>
+      <c r="AJ34">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="35" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI35">
+        <v>2.479166666666667</v>
+      </c>
+      <c r="AJ35">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="36" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI36">
+        <v>2.7083333333333339</v>
+      </c>
+      <c r="AJ36">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="37" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI37">
+        <v>2.916666666666667</v>
+      </c>
+      <c r="AJ37">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="38" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI38">
+        <v>0.66145833333333337</v>
+      </c>
+      <c r="AJ38">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="39" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI39">
+        <v>0.87916666666666665</v>
+      </c>
+      <c r="AJ39">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="40" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI40">
+        <v>1.3177083333333335</v>
+      </c>
+      <c r="AJ40">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="41" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI41">
+        <v>1.7416666666666667</v>
+      </c>
+      <c r="AJ41">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="42" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI42">
+        <v>1.9562499999999998</v>
+      </c>
+      <c r="AJ42">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="43" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI43">
+        <v>2.166666666666667</v>
+      </c>
+      <c r="AJ43">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="44" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI44">
+        <v>2.34375</v>
+      </c>
+      <c r="AJ44">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="45" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI45">
+        <v>2.5416666666666665</v>
+      </c>
+      <c r="AJ45">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="46" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI46">
+        <v>2.7395833333333335</v>
+      </c>
+      <c r="AJ46">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="47" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI47">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="AJ47">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="48" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI48">
+        <v>0.890625</v>
+      </c>
+      <c r="AJ48">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="49" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI49">
+        <v>1.3312500000000003</v>
+      </c>
+      <c r="AJ49">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="50" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI50">
+        <v>1.7677083333333334</v>
+      </c>
+      <c r="AJ50">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="51" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI51">
+        <v>1.9833333333333334</v>
+      </c>
+      <c r="AJ51">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="52" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI52">
+        <v>2.1875000000000004</v>
+      </c>
+      <c r="AJ52">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="53" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI53">
+        <v>2.385416666666667</v>
+      </c>
+      <c r="AJ53">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="54" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI54">
+        <v>2.59375</v>
+      </c>
+      <c r="AJ54">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="55" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI55">
+        <v>2.8020833333333335</v>
+      </c>
+      <c r="AJ55">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="56" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI56">
+        <v>0.6635416666666667</v>
+      </c>
+      <c r="AJ56">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="57" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI57">
+        <v>0.88437500000000002</v>
+      </c>
+      <c r="AJ57">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="58" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI58">
+        <v>1.3229166666666667</v>
+      </c>
+      <c r="AJ58">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="59" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI59">
+        <v>1.7593750000000004</v>
+      </c>
+      <c r="AJ59">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="60" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI60">
+        <v>1.9729166666666667</v>
+      </c>
+      <c r="AJ60">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="61" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI61">
+        <v>2.1770833333333335</v>
+      </c>
+      <c r="AJ61">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="62" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI62">
+        <v>2.3645833333333335</v>
+      </c>
+      <c r="AJ62">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="63" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI63">
+        <v>2.572916666666667</v>
+      </c>
+      <c r="AJ63">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="64" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI64">
+        <v>2.78125</v>
+      </c>
+      <c r="AJ64">
+        <v>39000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix solder SN7.  Recal SN2
</commit_message>
<xml_diff>
--- a/Saves/F2V_Cal20180104.xlsx
+++ b/Saves/F2V_Cal20180104.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary V4" sheetId="2" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>saturation, vrms.     Not measureable because signal generator does not produce enough voltage to satureate the LM2907/LM2917 device.</t>
   </si>
   <si>
-    <t>SN_0-1-3-4-5-5r-6_5</t>
-  </si>
-  <si>
     <t>uncertainties</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Data scatter +/-0.1 v@3</t>
+  </si>
+  <si>
+    <t>SN_ALL</t>
   </si>
 </sst>
 </file>
@@ -1254,11 +1254,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190499608"/>
-        <c:axId val="97464424"/>
+        <c:axId val="291012152"/>
+        <c:axId val="291015680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190499608"/>
+        <c:axId val="291012152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,12 +1338,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97464424"/>
+        <c:crossAx val="291015680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97464424"/>
+        <c:axId val="291015680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190499608"/>
+        <c:crossAx val="291012152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1532,7 +1532,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$Y$1</c:f>
+              <c:f>Data!$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1567,7 +1567,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1603,7 +1603,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Y$2:$Y$10</c:f>
+              <c:f>Data!$Z$2:$Z$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1644,7 +1644,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$Z$1</c:f>
+              <c:f>Data!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1679,7 +1679,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1715,7 +1715,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Z$2:$Z$10</c:f>
+              <c:f>Data!$AA$2:$AA$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1756,7 +1756,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AA$1</c:f>
+              <c:f>Data!$AB$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1791,7 +1791,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1827,36 +1827,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AA$2:$AA$10</c:f>
+              <c:f>Data!$AB$2:$AB$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.56222222222222218</c:v>
+                  <c:v>0.62655601659751037</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79777777777777781</c:v>
+                  <c:v>0.84751037344398328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2345555555555556</c:v>
+                  <c:v>1.2904564315352696</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7555555555555558</c:v>
+                  <c:v>1.7313278008298756</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8444444444444443</c:v>
+                  <c:v>1.9522821576763483</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.1680497925311202</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2888888888888888</c:v>
+                  <c:v>2.3858921161825721</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4666666666666668</c:v>
+                  <c:v>2.6037344398340245</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7</c:v>
+                  <c:v>2.8215767634854769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1868,7 +1868,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AB$1</c:f>
+              <c:f>Data!$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1903,7 +1903,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1939,7 +1939,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AB$2:$AB$10</c:f>
+              <c:f>Data!$AC$2:$AC$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1980,7 +1980,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AC$1</c:f>
+              <c:f>Data!$AD$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2015,7 +2015,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2051,7 +2051,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AC$2:$AC$10</c:f>
+              <c:f>Data!$AD$2:$AD$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2092,7 +2092,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AD$1</c:f>
+              <c:f>Data!$AE$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2127,7 +2127,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2163,7 +2163,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AD$2:$AD$10</c:f>
+              <c:f>Data!$AE$2:$AE$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2204,7 +2204,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AE$1</c:f>
+              <c:f>Data!$AF$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2245,7 +2245,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2281,7 +2281,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AE$2:$AE$10</c:f>
+              <c:f>Data!$AF$2:$AF$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2322,7 +2322,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AF$1</c:f>
+              <c:f>Data!$AG$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2363,7 +2363,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2399,7 +2399,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AF$2:$AF$10</c:f>
+              <c:f>Data!$AG$2:$AG$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2440,7 +2440,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$AG$1</c:f>
+              <c:f>Data!$AH$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2481,7 +2481,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$X$2:$X$10</c:f>
+              <c:f>Data!$Y$2:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2517,36 +2517,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AG$2:$AG$10</c:f>
+              <c:f>Data!$AH$2:$AH$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.60638297872340419</c:v>
+                  <c:v>0.65145228215767625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83191489361702131</c:v>
+                  <c:v>0.87136929460580914</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1489361702127661</c:v>
+                  <c:v>1.3112033195020747</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5702127659574465</c:v>
+                  <c:v>1.7510373443983402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.925531914893617</c:v>
+                  <c:v>1.9782157676348546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0957446808510638</c:v>
+                  <c:v>2.1887966804979251</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3617021276595747</c:v>
+                  <c:v>2.4170124481327799</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5106382978723403</c:v>
+                  <c:v>2.6244813278008294</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.6170212765957448</c:v>
+                  <c:v>2.8734439834024892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2561,11 +2561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="505695800"/>
-        <c:axId val="505691096"/>
+        <c:axId val="291012936"/>
+        <c:axId val="146263256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="505695800"/>
+        <c:axId val="291012936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2622,12 +2622,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505691096"/>
+        <c:crossAx val="146263256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="505691096"/>
+        <c:axId val="146263256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,7 +2684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505695800"/>
+        <c:crossAx val="291012936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3614,8 +3614,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="505696192"/>
-        <c:axId val="505695016"/>
+        <c:axId val="294162360"/>
+        <c:axId val="294168240"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -3756,7 +3756,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="505696192"/>
+        <c:axId val="294162360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3874,12 +3874,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505695016"/>
+        <c:crossAx val="294168240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="505695016"/>
+        <c:axId val="294168240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,7 +3999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505696192"/>
+        <c:crossAx val="294162360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4115,7 +4115,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Fit to SN 0, 1, 3, 4, 5, 5r, 6</a:t>
+              <a:t>Fit to  ALL</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4248,10 +4248,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$AI$2:$AI$73</c:f>
+              <c:f>Data!$AI$2:$AI$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>0.67187500000000011</c:v>
                 </c:pt>
@@ -4440,16 +4440,70 @@
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>2.78125</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.62655601659751037</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.84751037344398328</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.2904564315352696</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.7313278008298756</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.9522821576763483</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.1680497925311202</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.3858921161825721</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.6037344398340245</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.8215767634854769</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.65145228215767625</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.87136929460580914</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.3112033195020747</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.7510373443983402</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.9782157676348546</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.1887966804979251</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.4170124481327799</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.6244813278008294</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.8734439834024892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$AJ$2:$AJ$73</c:f>
+              <c:f>Data!$AJ$2:$AJ$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="72"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>9000</c:v>
                 </c:pt>
@@ -4637,6 +4691,60 @@
                   <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="62">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="80">
                   <c:v>39000</c:v>
                 </c:pt>
               </c:numCache>
@@ -4652,11 +4760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="519654760"/>
-        <c:axId val="509264856"/>
+        <c:axId val="294169024"/>
+        <c:axId val="294162752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="519654760"/>
+        <c:axId val="294169024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4769,12 +4877,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="509264856"/>
+        <c:crossAx val="294162752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="509264856"/>
+        <c:axId val="294162752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4892,7 +5000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="519654760"/>
+        <c:crossAx val="294169024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7169,7 +7277,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="65" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7180,7 +7288,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7191,7 +7299,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8648700" cy="6276975"/>
+    <xdr:ext cx="8663354" cy="6271846"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7218,7 +7326,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8648700" cy="6276975"/>
+    <xdr:ext cx="8663354" cy="6271846"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -7603,19 +7711,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9">
         <v>0.99975164058694566</v>
@@ -7623,7 +7731,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="9">
         <v>0.99950334285628939</v>
@@ -7631,7 +7739,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="9">
         <v>0.98337431059822489</v>
@@ -7639,7 +7747,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="9">
         <v>611.10893437582445</v>
@@ -7647,7 +7755,7 @@
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="10">
         <v>63</v>
@@ -7655,30 +7763,30 @@
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
@@ -7698,7 +7806,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="9">
         <v>62</v>
@@ -7714,7 +7822,7 @@
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="10">
         <v>63</v>
@@ -7730,33 +7838,33 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="9">
         <v>0</v>
@@ -7785,7 +7893,7 @@
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="10">
         <v>13632.38227201082</v>
@@ -7814,16 +7922,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -8340,10 +8448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ64"/>
+  <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AP8" sqref="AP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8354,8 +8462,8 @@
     <col min="4" max="4" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="12" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.88671875" style="1"/>
+    <col min="25" max="25" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" style="1"/>
     <col min="37" max="37" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22.21875" customWidth="1"/>
   </cols>
@@ -8430,38 +8538,39 @@
       <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="AI1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="AJ1" t="s">
         <v>12</v>
@@ -8521,7 +8630,7 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.50600000000000001</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="R2" s="1">
         <v>0.64800000000000002</v>
@@ -8539,46 +8648,47 @@
         <v>0.63700000000000001</v>
       </c>
       <c r="W2" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="X2" s="1">
+        <v>0.628</v>
+      </c>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1">
         <v>150</v>
       </c>
-      <c r="Y2" s="5">
-        <f t="shared" ref="Y2:Y10" si="0">O2/O$12*5</f>
+      <c r="Z2" s="5">
+        <f t="shared" ref="Z2:Z10" si="0">O2/O$12*5</f>
         <v>0.67187500000000011</v>
       </c>
-      <c r="Z2" s="5">
-        <f t="shared" ref="Z2:Z10" si="1">P2/P$12*5</f>
+      <c r="AA2" s="5">
+        <f t="shared" ref="AA2:AA10" si="1">P2/P$12*5</f>
         <v>0.68958333333333344</v>
       </c>
-      <c r="AA2" s="5">
-        <f t="shared" ref="AA2:AA10" si="2">Q2/Q$12*5</f>
-        <v>0.56222222222222218</v>
-      </c>
       <c r="AB2" s="5">
-        <f t="shared" ref="AB2:AB10" si="3">R2/R$12*5</f>
+        <f t="shared" ref="AB2:AB10" si="2">Q2/Q$12*5</f>
+        <v>0.62655601659751037</v>
+      </c>
+      <c r="AC2" s="5">
+        <f t="shared" ref="AC2:AC10" si="3">R2/R$12*5</f>
         <v>0.67500000000000004</v>
       </c>
-      <c r="AC2" s="5">
-        <f t="shared" ref="AC2:AC10" si="4">S2/S$12*5</f>
+      <c r="AD2" s="5">
+        <f t="shared" ref="AD2:AD10" si="4">S2/S$12*5</f>
         <v>0.69062500000000016</v>
       </c>
-      <c r="AD2" s="5">
-        <f t="shared" ref="AD2:AD10" si="5">T2/T$12*5</f>
+      <c r="AE2" s="5">
+        <f t="shared" ref="AE2:AE10" si="5">T2/T$12*5</f>
         <v>0.66145833333333337</v>
       </c>
-      <c r="AE2" s="5">
-        <f t="shared" ref="AE2:AE10" si="6">U2/U$12*5</f>
+      <c r="AF2" s="5">
+        <f t="shared" ref="AF2:AF10" si="6">U2/U$12*5</f>
         <v>0.67083333333333339</v>
       </c>
-      <c r="AF2" s="5">
-        <f t="shared" ref="AF2:AF10" si="7">V2/V$12*5</f>
+      <c r="AG2" s="5">
+        <f t="shared" ref="AG2:AG10" si="7">V2/V$12*5</f>
         <v>0.6635416666666667</v>
       </c>
-      <c r="AG2" s="5">
-        <f t="shared" ref="AG2:AG10" si="8">W2/W$12*5</f>
-        <v>0.60638297872340419</v>
+      <c r="AH2" s="5">
+        <f t="shared" ref="AH2:AH10" si="8">W2/W$12*5</f>
+        <v>0.65145228215767625</v>
       </c>
       <c r="AI2">
         <v>0.67187500000000011</v>
@@ -8590,14 +8700,14 @@
         <v>13</v>
       </c>
       <c r="AL2" s="2">
-        <f>INDEX(LINEST($AJ$2:$AJ$64,AI$2:AI$64^{1,2},FALSE,FALSE),3)</f>
+        <f>INDEX(LINEST($AJ$2:$AJ$82,AI$2:AI$82^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
       </c>
       <c r="AO2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AQ2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
@@ -8652,7 +8762,7 @@
         <v>0.88400000000000001</v>
       </c>
       <c r="Q3" s="1">
-        <v>0.71799999999999997</v>
+        <v>0.81699999999999995</v>
       </c>
       <c r="R3" s="1">
         <v>0.86399999999999999</v>
@@ -8670,46 +8780,47 @@
         <v>0.84899999999999998</v>
       </c>
       <c r="W3" s="1">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="X3" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1">
         <v>200</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Z3" s="5">
         <f t="shared" si="0"/>
         <v>0.89687500000000009</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="AA3" s="5">
         <f t="shared" si="1"/>
         <v>0.92083333333333339</v>
       </c>
-      <c r="AA3" s="5">
+      <c r="AB3" s="5">
         <f t="shared" si="2"/>
-        <v>0.79777777777777781</v>
-      </c>
-      <c r="AB3" s="5">
+        <v>0.84751037344398328</v>
+      </c>
+      <c r="AC3" s="5">
         <f t="shared" si="3"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AD3" s="5">
         <f t="shared" si="4"/>
         <v>0.921875</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AE3" s="5">
         <f t="shared" si="5"/>
         <v>0.87916666666666665</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AF3" s="5">
         <f t="shared" si="6"/>
         <v>0.890625</v>
       </c>
-      <c r="AF3" s="5">
+      <c r="AG3" s="5">
         <f t="shared" si="7"/>
         <v>0.88437500000000002</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AH3" s="5">
         <f t="shared" si="8"/>
-        <v>0.83191489361702131</v>
+        <v>0.87136929460580914</v>
       </c>
       <c r="AI3">
         <v>0.89687500000000009</v>
@@ -8721,11 +8832,11 @@
         <v>14</v>
       </c>
       <c r="AL3" s="2">
-        <f>INDEX(LINEST($AJ$2:$AJ$64,AI$2:AI$64^{1,2},FALSE,FALSE),2)</f>
-        <v>13075.140888643438</v>
+        <f>INDEX(LINEST($AJ$2:$AJ$82,AI$2:AI$82^{1,2},FALSE,FALSE),2)</f>
+        <v>13281.961358003236</v>
       </c>
       <c r="AP3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AQ3" s="8">
         <f>0.1/5*100</f>
@@ -8784,7 +8895,7 @@
         <v>1.32</v>
       </c>
       <c r="Q4" s="1">
-        <v>1.1111</v>
+        <v>1.244</v>
       </c>
       <c r="R4" s="1">
         <v>1.2929999999999999</v>
@@ -8802,46 +8913,47 @@
         <v>1.27</v>
       </c>
       <c r="W4" s="1">
-        <v>1.08</v>
-      </c>
-      <c r="X4" s="1">
+        <v>1.264</v>
+      </c>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1">
         <v>300</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Z4" s="5">
         <f t="shared" si="0"/>
         <v>1.3427083333333334</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="AA4" s="5">
         <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
-      <c r="AA4" s="5">
+      <c r="AB4" s="5">
         <f t="shared" si="2"/>
-        <v>1.2345555555555556</v>
-      </c>
-      <c r="AB4" s="5">
+        <v>1.2904564315352696</v>
+      </c>
+      <c r="AC4" s="5">
         <f t="shared" si="3"/>
         <v>1.3468749999999998</v>
       </c>
-      <c r="AC4" s="5">
+      <c r="AD4" s="5">
         <f t="shared" si="4"/>
         <v>1.3791666666666669</v>
       </c>
-      <c r="AD4" s="5">
+      <c r="AE4" s="5">
         <f t="shared" si="5"/>
         <v>1.3177083333333335</v>
       </c>
-      <c r="AE4" s="5">
+      <c r="AF4" s="5">
         <f t="shared" si="6"/>
         <v>1.3312500000000003</v>
       </c>
-      <c r="AF4" s="5">
+      <c r="AG4" s="5">
         <f t="shared" si="7"/>
         <v>1.3229166666666667</v>
       </c>
-      <c r="AG4" s="5">
+      <c r="AH4" s="5">
         <f t="shared" si="8"/>
-        <v>1.1489361702127661</v>
+        <v>1.3112033195020747</v>
       </c>
       <c r="AI4">
         <v>1.3427083333333334</v>
@@ -8853,11 +8965,11 @@
         <v>15</v>
       </c>
       <c r="AL4" s="2">
-        <f>INDEX(LINEST($AJ$2:$AJ$64,AI$2:AI$64^{1,2},FALSE,FALSE),1)</f>
-        <v>241.69450165398891</v>
+        <f>INDEX(LINEST($AJ$2:$AJ$82,AI$2:AI$82^{1,2},FALSE,FALSE),1)</f>
+        <v>163.82242834703445</v>
       </c>
       <c r="AP4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AQ4" s="8">
         <f>0.1/3*100</f>
@@ -8918,7 +9030,7 @@
         <v>1.76</v>
       </c>
       <c r="Q5" s="1">
-        <v>1.58</v>
+        <v>1.669</v>
       </c>
       <c r="R5" s="1">
         <v>1.72</v>
@@ -8936,52 +9048,56 @@
         <v>1.6890000000000001</v>
       </c>
       <c r="W5" s="1">
-        <v>1.476</v>
-      </c>
-      <c r="X5" s="1">
+        <v>1.6879999999999999</v>
+      </c>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1">
         <v>400</v>
       </c>
-      <c r="Y5" s="5">
+      <c r="Z5" s="5">
         <f t="shared" si="0"/>
         <v>1.78125</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="AA5" s="5">
         <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
-      <c r="AA5" s="5">
+      <c r="AB5" s="5">
         <f t="shared" si="2"/>
-        <v>1.7555555555555558</v>
-      </c>
-      <c r="AB5" s="5">
+        <v>1.7313278008298756</v>
+      </c>
+      <c r="AC5" s="5">
         <f t="shared" si="3"/>
         <v>1.7916666666666667</v>
       </c>
-      <c r="AC5" s="5">
+      <c r="AD5" s="5">
         <f t="shared" si="4"/>
         <v>1.8333333333333335</v>
       </c>
-      <c r="AD5" s="5">
+      <c r="AE5" s="5">
         <f t="shared" si="5"/>
         <v>1.7416666666666667</v>
       </c>
-      <c r="AE5" s="5">
+      <c r="AF5" s="5">
         <f t="shared" si="6"/>
         <v>1.7677083333333334</v>
       </c>
-      <c r="AF5" s="5">
+      <c r="AG5" s="5">
         <f t="shared" si="7"/>
         <v>1.7593750000000004</v>
       </c>
-      <c r="AG5" s="5">
+      <c r="AH5" s="5">
         <f t="shared" si="8"/>
-        <v>1.5702127659574465</v>
+        <v>1.7510373443983402</v>
       </c>
       <c r="AI5">
         <v>1.78125</v>
       </c>
       <c r="AJ5">
         <v>24000</v>
+      </c>
+      <c r="AN5">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
@@ -9036,7 +9152,7 @@
         <v>1.96</v>
       </c>
       <c r="Q6" s="1">
-        <v>1.66</v>
+        <v>1.8819999999999999</v>
       </c>
       <c r="R6" s="1">
         <v>1.92</v>
@@ -9054,46 +9170,47 @@
         <v>1.8939999999999999</v>
       </c>
       <c r="W6" s="1">
-        <v>1.81</v>
-      </c>
-      <c r="X6" s="1">
+        <v>1.907</v>
+      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1">
         <v>450</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Z6" s="5">
         <f t="shared" si="0"/>
         <v>1.9895833333333333</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="AA6" s="5">
         <f t="shared" si="1"/>
         <v>2.0416666666666665</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AB6" s="5">
         <f t="shared" si="2"/>
-        <v>1.8444444444444443</v>
-      </c>
-      <c r="AB6" s="5">
+        <v>1.9522821576763483</v>
+      </c>
+      <c r="AC6" s="5">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="AC6" s="5">
+      <c r="AD6" s="5">
         <f t="shared" si="4"/>
         <v>2.052083333333333</v>
       </c>
-      <c r="AD6" s="5">
+      <c r="AE6" s="5">
         <f t="shared" si="5"/>
         <v>1.9562499999999998</v>
       </c>
-      <c r="AE6" s="5">
+      <c r="AF6" s="5">
         <f t="shared" si="6"/>
         <v>1.9833333333333334</v>
       </c>
-      <c r="AF6" s="5">
+      <c r="AG6" s="5">
         <f t="shared" si="7"/>
         <v>1.9729166666666667</v>
       </c>
-      <c r="AG6" s="5">
+      <c r="AH6" s="5">
         <f t="shared" si="8"/>
-        <v>1.925531914893617</v>
+        <v>1.9782157676348546</v>
       </c>
       <c r="AI6">
         <v>1.9895833333333333</v>
@@ -9154,7 +9271,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="Q7" s="1">
-        <v>1.9</v>
+        <v>2.09</v>
       </c>
       <c r="R7" s="1">
         <v>2.13</v>
@@ -9172,46 +9289,47 @@
         <v>2.09</v>
       </c>
       <c r="W7" s="1">
-        <v>1.97</v>
-      </c>
-      <c r="X7" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1">
         <v>500</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="Z7" s="5">
         <f t="shared" si="0"/>
         <v>2.2083333333333335</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="AA7" s="5">
         <f t="shared" si="1"/>
         <v>2.2708333333333335</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AB7" s="5">
         <f t="shared" si="2"/>
-        <v>2.1111111111111112</v>
-      </c>
-      <c r="AB7" s="5">
+        <v>2.1680497925311202</v>
+      </c>
+      <c r="AC7" s="5">
         <f t="shared" si="3"/>
         <v>2.21875</v>
       </c>
-      <c r="AC7" s="5">
+      <c r="AD7" s="5">
         <f t="shared" si="4"/>
         <v>2.2708333333333335</v>
       </c>
-      <c r="AD7" s="5">
+      <c r="AE7" s="5">
         <f t="shared" si="5"/>
         <v>2.166666666666667</v>
       </c>
-      <c r="AE7" s="5">
+      <c r="AF7" s="5">
         <f t="shared" si="6"/>
         <v>2.1875000000000004</v>
       </c>
-      <c r="AF7" s="5">
+      <c r="AG7" s="5">
         <f t="shared" si="7"/>
         <v>2.1770833333333335</v>
       </c>
-      <c r="AG7" s="5">
+      <c r="AH7" s="5">
         <f t="shared" si="8"/>
-        <v>2.0957446808510638</v>
+        <v>2.1887966804979251</v>
       </c>
       <c r="AI7">
         <v>2.2083333333333335</v>
@@ -9272,7 +9390,7 @@
         <v>2.37</v>
       </c>
       <c r="Q8" s="1">
-        <v>2.06</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="R8" s="1">
         <v>2.33</v>
@@ -9290,46 +9408,47 @@
         <v>2.27</v>
       </c>
       <c r="W8" s="1">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="X8" s="1">
+        <v>2.33</v>
+      </c>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1">
         <v>550</v>
       </c>
-      <c r="Y8" s="5">
+      <c r="Z8" s="5">
         <f t="shared" si="0"/>
         <v>2.395833333333333</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="AA8" s="5">
         <f t="shared" si="1"/>
         <v>2.46875</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AB8" s="5">
         <f t="shared" si="2"/>
-        <v>2.2888888888888888</v>
-      </c>
-      <c r="AB8" s="5">
+        <v>2.3858921161825721</v>
+      </c>
+      <c r="AC8" s="5">
         <f t="shared" si="3"/>
         <v>2.4270833333333335</v>
       </c>
-      <c r="AC8" s="5">
+      <c r="AD8" s="5">
         <f t="shared" si="4"/>
         <v>2.479166666666667</v>
       </c>
-      <c r="AD8" s="5">
+      <c r="AE8" s="5">
         <f t="shared" si="5"/>
         <v>2.34375</v>
       </c>
-      <c r="AE8" s="5">
+      <c r="AF8" s="5">
         <f t="shared" si="6"/>
         <v>2.385416666666667</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AG8" s="5">
         <f t="shared" si="7"/>
         <v>2.3645833333333335</v>
       </c>
-      <c r="AG8" s="5">
+      <c r="AH8" s="5">
         <f t="shared" si="8"/>
-        <v>2.3617021276595747</v>
+        <v>2.4170124481327799</v>
       </c>
       <c r="AI8">
         <v>2.395833333333333</v>
@@ -9392,7 +9511,7 @@
         <v>2.59</v>
       </c>
       <c r="Q9" s="1">
-        <v>2.2200000000000002</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="R9" s="1">
         <v>2.5299999999999998</v>
@@ -9410,46 +9529,47 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="W9" s="1">
-        <v>2.36</v>
-      </c>
-      <c r="X9" s="1">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1">
         <v>600</v>
       </c>
-      <c r="Y9" s="5">
+      <c r="Z9" s="5">
         <f t="shared" si="0"/>
         <v>2.6145833333333335</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="AA9" s="5">
         <f t="shared" si="1"/>
         <v>2.6979166666666665</v>
       </c>
-      <c r="AA9" s="5">
+      <c r="AB9" s="5">
         <f t="shared" si="2"/>
-        <v>2.4666666666666668</v>
-      </c>
-      <c r="AB9" s="5">
+        <v>2.6037344398340245</v>
+      </c>
+      <c r="AC9" s="5">
         <f t="shared" si="3"/>
         <v>2.635416666666667</v>
       </c>
-      <c r="AC9" s="5">
+      <c r="AD9" s="5">
         <f t="shared" si="4"/>
         <v>2.7083333333333339</v>
       </c>
-      <c r="AD9" s="5">
+      <c r="AE9" s="5">
         <f t="shared" si="5"/>
         <v>2.5416666666666665</v>
       </c>
-      <c r="AE9" s="5">
+      <c r="AF9" s="5">
         <f t="shared" si="6"/>
         <v>2.59375</v>
       </c>
-      <c r="AF9" s="5">
+      <c r="AG9" s="5">
         <f t="shared" si="7"/>
         <v>2.572916666666667</v>
       </c>
-      <c r="AG9" s="5">
+      <c r="AH9" s="5">
         <f t="shared" si="8"/>
-        <v>2.5106382978723403</v>
+        <v>2.6244813278008294</v>
       </c>
       <c r="AI9">
         <v>2.6145833333333335</v>
@@ -9510,7 +9630,7 @@
         <v>2.77</v>
       </c>
       <c r="Q10" s="1">
-        <v>2.4300000000000002</v>
+        <v>2.72</v>
       </c>
       <c r="R10" s="1">
         <v>2.69</v>
@@ -9528,46 +9648,47 @@
         <v>2.67</v>
       </c>
       <c r="W10" s="1">
-        <v>2.46</v>
-      </c>
-      <c r="X10" s="1">
+        <v>2.77</v>
+      </c>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1">
         <v>650</v>
       </c>
-      <c r="Y10" s="5">
+      <c r="Z10" s="5">
         <f t="shared" si="0"/>
         <v>2.8125000000000004</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="AA10" s="5">
         <f t="shared" si="1"/>
         <v>2.885416666666667</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AB10" s="5">
         <f t="shared" si="2"/>
-        <v>2.7</v>
-      </c>
-      <c r="AB10" s="5">
+        <v>2.8215767634854769</v>
+      </c>
+      <c r="AC10" s="5">
         <f t="shared" si="3"/>
         <v>2.8020833333333335</v>
       </c>
-      <c r="AC10" s="5">
+      <c r="AD10" s="5">
         <f t="shared" si="4"/>
         <v>2.916666666666667</v>
       </c>
-      <c r="AD10" s="5">
+      <c r="AE10" s="5">
         <f t="shared" si="5"/>
         <v>2.7395833333333335</v>
       </c>
-      <c r="AE10" s="5">
+      <c r="AF10" s="5">
         <f t="shared" si="6"/>
         <v>2.8020833333333335</v>
       </c>
-      <c r="AF10" s="5">
+      <c r="AG10" s="5">
         <f t="shared" si="7"/>
         <v>2.78125</v>
       </c>
-      <c r="AG10" s="5">
+      <c r="AH10" s="5">
         <f t="shared" si="8"/>
-        <v>2.6170212765957448</v>
+        <v>2.8734439834024892</v>
       </c>
       <c r="AI10">
         <v>2.8125000000000004</v>
@@ -9598,7 +9719,7 @@
         <v>4.8</v>
       </c>
       <c r="Q12" s="1">
-        <v>4.5</v>
+        <v>4.82</v>
       </c>
       <c r="R12" s="1">
         <v>4.8</v>
@@ -9616,8 +9737,9 @@
         <v>4.8</v>
       </c>
       <c r="W12" s="1">
-        <v>4.7</v>
-      </c>
+        <v>4.82</v>
+      </c>
+      <c r="X12" s="1"/>
       <c r="AI12">
         <v>0.92083333333333339</v>
       </c>
@@ -9645,6 +9767,7 @@
       <c r="W13" s="1">
         <v>98000</v>
       </c>
+      <c r="X13" s="1"/>
       <c r="AI13">
         <v>1.375</v>
       </c>
@@ -9689,10 +9812,6 @@
         <v>0</v>
       </c>
       <c r="T14" s="1"/>
-      <c r="Y14" s="2">
-        <f>INDEX(LINEST($N$2:$N$10,Y$2:Y$10^{1,2},FALSE,FALSE),3)</f>
-        <v>0</v>
-      </c>
       <c r="Z14" s="2">
         <f>INDEX(LINEST($N$2:$N$10,Z$2:Z$10^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
@@ -9723,6 +9842,10 @@
       </c>
       <c r="AG14" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AG$2:AG$10^{1,2},FALSE,FALSE),3)</f>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,AH$2:AH$10^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
       </c>
       <c r="AI14">
@@ -9774,41 +9897,41 @@
         <v>12709.700509362918</v>
       </c>
       <c r="T15" s="1"/>
-      <c r="Y15" s="2">
-        <f>INDEX(LINEST($N$2:$N$10,Y$2:Y$10^{1,2},FALSE,FALSE),2)</f>
-        <v>13001.51518426758</v>
-      </c>
       <c r="Z15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,Z$2:Z$10^{1,2},FALSE,FALSE),2)</f>
-        <v>12682.035489514199</v>
+        <v>13001.51518426758</v>
       </c>
       <c r="AA15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AA$2:AA$10^{1,2},FALSE,FALSE),2)</f>
-        <v>14542.538394794556</v>
+        <v>12682.035489514199</v>
       </c>
       <c r="AB15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AB$2:AB$10^{1,2},FALSE,FALSE),2)</f>
-        <v>12866.208103938689</v>
+        <v>14111.034872877302</v>
       </c>
       <c r="AC15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AC$2:AC$10^{1,2},FALSE,FALSE),2)</f>
-        <v>12772.560908129319</v>
+        <v>12866.208103938689</v>
       </c>
       <c r="AD15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AD$2:AD$10^{1,2},FALSE,FALSE),2)</f>
-        <v>13108.876059633149</v>
+        <v>12772.560908129319</v>
       </c>
       <c r="AE15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AE$2:AE$10^{1,2},FALSE,FALSE),2)</f>
-        <v>13114.798359155298</v>
+        <v>13108.876059633149</v>
       </c>
       <c r="AF15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AF$2:AF$10^{1,2},FALSE,FALSE),2)</f>
-        <v>13166.023073080518</v>
+        <v>13114.798359155298</v>
       </c>
       <c r="AG15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AG$2:AG$10^{1,2},FALSE,FALSE),2)</f>
-        <v>15136.749829040513</v>
+        <v>13166.023073080518</v>
+      </c>
+      <c r="AH15" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,AH$2:AH$10^{1,2},FALSE,FALSE),2)</f>
+        <v>13848.123238227665</v>
       </c>
       <c r="AI15">
         <v>2.0416666666666665</v>
@@ -9859,41 +9982,41 @@
         <v>84.174995967615558</v>
       </c>
       <c r="T16" s="1"/>
-      <c r="Y16" s="2">
-        <f>INDEX(LINEST($N$2:$N$10,Y$2:Y$10^{1,2},FALSE,FALSE),1)</f>
-        <v>298.10803865471041</v>
-      </c>
       <c r="Z16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,Z$2:Z$10^{1,2},FALSE,FALSE),1)</f>
-        <v>265.14715738785526</v>
+        <v>298.10803865471041</v>
       </c>
       <c r="AA16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AA$2:AA$10^{1,2},FALSE,FALSE),1)</f>
-        <v>-57.642391115915849</v>
+        <v>265.14715738785526</v>
       </c>
       <c r="AB16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AB$2:AB$10^{1,2},FALSE,FALSE),1)</f>
-        <v>326.60580357888693</v>
+        <v>-113.97783034536754</v>
       </c>
       <c r="AC16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AC$2:AC$10^{1,2},FALSE,FALSE),1)</f>
-        <v>199.95323366264739</v>
+        <v>326.60580357888693</v>
       </c>
       <c r="AD16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AD$2:AD$10^{1,2},FALSE,FALSE),1)</f>
-        <v>399.04974198141809</v>
+        <v>199.95323366264739</v>
       </c>
       <c r="AE16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AE$2:AE$10^{1,2},FALSE,FALSE),1)</f>
-        <v>286.34030014894239</v>
+        <v>399.04974198141809</v>
       </c>
       <c r="AF16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AF$2:AF$10^{1,2},FALSE,FALSE),1)</f>
-        <v>307.87371513414195</v>
+        <v>286.34030014894239</v>
       </c>
       <c r="AG16" s="2">
         <f>INDEX(LINEST($N$2:$N$10,AG$2:AG$10^{1,2},FALSE,FALSE),1)</f>
-        <v>-293.79797147707922</v>
+        <v>307.87371513414195</v>
+      </c>
+      <c r="AH16" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,AH$2:AH$10^{1,2},FALSE,FALSE),1)</f>
+        <v>-78.489029824631501</v>
       </c>
       <c r="AI16">
         <v>2.2708333333333335</v>
@@ -10342,6 +10465,150 @@
         <v>39000</v>
       </c>
     </row>
+    <row r="65" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI65">
+        <v>0.62655601659751037</v>
+      </c>
+      <c r="AJ65">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="66" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI66">
+        <v>0.84751037344398328</v>
+      </c>
+      <c r="AJ66">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="67" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI67">
+        <v>1.2904564315352696</v>
+      </c>
+      <c r="AJ67">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="68" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI68">
+        <v>1.7313278008298756</v>
+      </c>
+      <c r="AJ68">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="69" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI69">
+        <v>1.9522821576763483</v>
+      </c>
+      <c r="AJ69">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="70" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI70">
+        <v>2.1680497925311202</v>
+      </c>
+      <c r="AJ70">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="71" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI71">
+        <v>2.3858921161825721</v>
+      </c>
+      <c r="AJ71">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="72" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI72">
+        <v>2.6037344398340245</v>
+      </c>
+      <c r="AJ72">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="73" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI73">
+        <v>2.8215767634854769</v>
+      </c>
+      <c r="AJ73">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="74" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI74">
+        <v>0.65145228215767625</v>
+      </c>
+      <c r="AJ74">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="75" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI75">
+        <v>0.87136929460580914</v>
+      </c>
+      <c r="AJ75">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="76" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI76">
+        <v>1.3112033195020747</v>
+      </c>
+      <c r="AJ76">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="77" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI77">
+        <v>1.7510373443983402</v>
+      </c>
+      <c r="AJ77">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="78" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI78">
+        <v>1.9782157676348546</v>
+      </c>
+      <c r="AJ78">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="79" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI79">
+        <v>2.1887966804979251</v>
+      </c>
+      <c r="AJ79">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="80" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI80">
+        <v>2.4170124481327799</v>
+      </c>
+      <c r="AJ80">
+        <v>33000</v>
+      </c>
+    </row>
+    <row r="81" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI81">
+        <v>2.6244813278008294</v>
+      </c>
+      <c r="AJ81">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="82" spans="35:36" x14ac:dyDescent="0.3">
+      <c r="AI82">
+        <v>2.8734439834024892</v>
+      </c>
+      <c r="AJ82">
+        <v>39000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>